<commit_message>
Added the excel file
</commit_message>
<xml_diff>
--- a/data/Groups.xlsx
+++ b/data/Groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohitm\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C36715E9-E31F-4A35-B448-B257365C5465}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{748D1C8E-7AC4-459C-B325-1485E180A6FC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{F5DA3433-3288-47F3-8B87-500588D53752}" yWindow="-120"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Group</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Business Name</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ends with</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -418,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD1C965-25A0-4170-BB64-5E88DC0DD19E}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,10 +487,21 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Done Editing scenarios 2.Done verification of OR/AND connection 3. Done initial deletion
</commit_message>
<xml_diff>
--- a/data/Groups.xlsx
+++ b/data/Groups.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohitm\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{748D1C8E-7AC4-459C-B325-1485E180A6FC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E9A4380F-827E-4399-B17D-82C92671DDC8}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{F5DA3433-3288-47F3-8B87-500588D53752}" yWindow="-120"/>
+    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{F5DA3433-3288-47F3-8B87-500588D53752}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Group</t>
   </si>
@@ -81,6 +82,39 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Country_Group_A</t>
+  </si>
+  <si>
+    <t>Countries name starting with A</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>does not end with</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Report Group</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>AND</t>
   </si>
 </sst>
 </file>
@@ -433,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD1C965-25A0-4170-BB64-5E88DC0DD19E}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,9 +480,10 @@
     <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +499,11 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -481,8 +519,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -492,8 +533,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -508,4 +552,92 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B825998-7BDD-4224-A8EA-B73730828216}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="51.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code in Groups page
</commit_message>
<xml_diff>
--- a/data/Groups.xlsx
+++ b/data/Groups.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohitm\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{E9A4380F-827E-4399-B17D-82C92671DDC8}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B4EB04F9-7B47-4FBB-8EE7-5CCC6414A672}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{F5DA3433-3288-47F3-8B87-500588D53752}" yWindow="-120"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Group</t>
   </si>
@@ -57,64 +57,61 @@
     <t>Country_Group_N</t>
   </si>
   <si>
+    <t>starts with</t>
+  </si>
+  <si>
+    <t>Business Name</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ends with</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Country_Group_A</t>
+  </si>
+  <si>
+    <t>Countries name starting with A</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>does not end with</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Report Group</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Location Number</t>
-  </si>
-  <si>
-    <t>starts with</t>
-  </si>
-  <si>
-    <t>Business Name</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>contains</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>ends with</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Country_Group_A</t>
-  </si>
-  <si>
-    <t>Countries name starting with A</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>does not end with</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Report Group</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>AND</t>
+    <t>Postal Code</t>
   </si>
 </sst>
 </file>
@@ -470,7 +467,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -511,41 +508,41 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +556,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,52 +586,52 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>